<commit_message>
a varible is decleared
</commit_message>
<xml_diff>
--- a/realstatedata.xlsx
+++ b/realstatedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Phone Numbers</t>
   </si>
@@ -37,127 +37,184 @@
     <t>Business Name</t>
   </si>
   <si>
-    <t>(208) 327-4800, (208) 524-5511, (801) 433-3663</t>
-  </si>
-  <si>
-    <t>(253) 851-7424, (425) 251-4988</t>
-  </si>
-  <si>
-    <t>(219) 879-9083</t>
-  </si>
-  <si>
-    <t>(813) 488-5114</t>
-  </si>
-  <si>
-    <t>(419) 464-7660</t>
-  </si>
-  <si>
-    <t>744 E 400 S</t>
-  </si>
-  <si>
-    <t>555 Jefferson St</t>
-  </si>
-  <si>
-    <t>14320 92nd Ave Nw</t>
-  </si>
-  <si>
-    <t>6466 W Johnson Rd</t>
-  </si>
-  <si>
-    <t>6467 US Highway 301 S</t>
-  </si>
-  <si>
-    <t>1923 W Alexis</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Lafayette</t>
-  </si>
-  <si>
-    <t>Wauna</t>
-  </si>
-  <si>
-    <t>LaPorte</t>
-  </si>
-  <si>
-    <t>Riverview</t>
-  </si>
-  <si>
-    <t>Toledo</t>
+    <t>(925) 398-8184</t>
+  </si>
+  <si>
+    <t>(360) 609-5291, (360) 727-5975</t>
+  </si>
+  <si>
+    <t>(916) 243-3189, (916) 812-8586</t>
+  </si>
+  <si>
+    <t>(310) 717-8152</t>
+  </si>
+  <si>
+    <t>(773) 983-8635</t>
+  </si>
+  <si>
+    <t>(951) 283-4370</t>
+  </si>
+  <si>
+    <t>(559) 840-5603</t>
+  </si>
+  <si>
+    <t>(541) 206-9865, (541) 683-3606</t>
+  </si>
+  <si>
+    <t>(510) 812-9629, (510) 527-1219</t>
+  </si>
+  <si>
+    <t>5673 W Las Positas Blvd Ste 203</t>
+  </si>
+  <si>
+    <t>7208 NE 101st St Ste A</t>
+  </si>
+  <si>
+    <t>1151 Pacific Ave</t>
+  </si>
+  <si>
+    <t>820 S Holt Ave</t>
+  </si>
+  <si>
+    <t>980 Teton Dr</t>
+  </si>
+  <si>
+    <t>1749 Bern Dr</t>
+  </si>
+  <si>
+    <t>800 E 11600 S</t>
+  </si>
+  <si>
+    <t>PO Box 3051</t>
+  </si>
+  <si>
+    <t>106 E 16th Ave</t>
+  </si>
+  <si>
+    <t>379 Vassar Ave</t>
+  </si>
+  <si>
+    <t>Pleasanton</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>Rio Oso</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>Corona</t>
+  </si>
+  <si>
+    <t>Draper</t>
+  </si>
+  <si>
+    <t>Fresno</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>Berkeley</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>IL</t>
   </si>
   <si>
     <t>UT</t>
   </si>
   <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>84102-2902</t>
-  </si>
-  <si>
-    <t>70501-6905</t>
-  </si>
-  <si>
-    <t>98329</t>
-  </si>
-  <si>
-    <t>46350</t>
-  </si>
-  <si>
-    <t>33578</t>
-  </si>
-  <si>
-    <t>43613</t>
-  </si>
-  <si>
-    <t>http://www.chuck-a-rama.com</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/Vestal-Restaurant-105838060945532/</t>
-  </si>
-  <si>
-    <t>https://www.bk.com/store-locator/store/restaurant_9116</t>
-  </si>
-  <si>
-    <t>https://waterfordinnlaporte.com/</t>
-  </si>
-  <si>
-    <t>https://www.flavazjamaicangrille.com/</t>
-  </si>
-  <si>
-    <t>https://sip-and-brew.square.site/</t>
-  </si>
-  <si>
-    <t>Chuck-A-Rama Buffet</t>
-  </si>
-  <si>
-    <t>Vestal Restaurant, LLC</t>
-  </si>
-  <si>
-    <t>Ambrosia QSR Burger, LLC</t>
-  </si>
-  <si>
-    <t>Waterford Inn II</t>
-  </si>
-  <si>
-    <t>Flavaz Jamaican Grille</t>
-  </si>
-  <si>
-    <t>Sip and Brew</t>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>94588-4077</t>
+  </si>
+  <si>
+    <t>98662</t>
+  </si>
+  <si>
+    <t>95674-9618</t>
+  </si>
+  <si>
+    <t>90035-1807</t>
+  </si>
+  <si>
+    <t>60098-6503</t>
+  </si>
+  <si>
+    <t>92882-4754</t>
+  </si>
+  <si>
+    <t>84020-9392</t>
+  </si>
+  <si>
+    <t>93650-3051</t>
+  </si>
+  <si>
+    <t>97401</t>
+  </si>
+  <si>
+    <t>94708-1251</t>
+  </si>
+  <si>
+    <t>https://www.yelp.com/biz/cal-coast-window-and-door-danville, https://calcoastwindows.com/, https://www.thumbtack.com/ca/pleasanton/window-installation/cal-coast-window-door/service/286325850029556784</t>
+  </si>
+  <si>
+    <t>https://wearegro.com/, http://www.grooutdoorliving.com/</t>
+  </si>
+  <si>
+    <t>http://www.mazza-homes.com</t>
+  </si>
+  <si>
+    <t>http://www.adasbasement.com</t>
+  </si>
+  <si>
+    <t>https://damiandelappbuilders.com</t>
+  </si>
+  <si>
+    <t>https://www.bureaumembers.com/betterrooterplumbing/, https://www.yelp.com/biz/a-better-rooter-plumbing-and-engineering-berkeley</t>
+  </si>
+  <si>
+    <t>Cal Coast Window &amp; Door</t>
+  </si>
+  <si>
+    <t>Gro Outdoor Living</t>
+  </si>
+  <si>
+    <t>Mazza Homes</t>
+  </si>
+  <si>
+    <t>Power Air and Fire</t>
+  </si>
+  <si>
+    <t>Adas Interior Remodeling, Inc.</t>
+  </si>
+  <si>
+    <t>Damian Delapp Builders</t>
+  </si>
+  <si>
+    <t>C R Tafoya &amp; Company</t>
+  </si>
+  <si>
+    <t>J S Construction</t>
+  </si>
+  <si>
+    <t>Creative Contractor Solutions LLC</t>
+  </si>
+  <si>
+    <t>A Better Rooter Plumbing</t>
   </si>
 </sst>
 </file>
@@ -528,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -562,134 +619,214 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -697,9 +834,9 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>